<commit_message>
Job seeker BRD and Solution is done - Preet and Raji.
</commit_message>
<xml_diff>
--- a/8hourjobs_BRD_Solution_TC_Raji.xlsx
+++ b/8hourjobs_BRD_Solution_TC_Raji.xlsx
@@ -303,9 +303,6 @@
     <t>Registration page</t>
   </si>
   <si>
-    <t>After data's stored in the database. An E-mail should be sent to Job seeker's E-mail ID. Job seeker should navigate to profile page</t>
-  </si>
-  <si>
     <t>Sign In / Login</t>
   </si>
   <si>
@@ -487,9 +484,6 @@
   </si>
   <si>
     <t>Suburb</t>
-  </si>
-  <si>
-    <t>By default display "Please select suburb".  If not selected any suburb display error as "Select suburb from list".</t>
   </si>
   <si>
     <t>The register button triggers the validation based on the Field No Sequence. IF there is a problem :  At one point of time it will display only one error message for the first incorrect field value identified by the logic. Error message should be red in colour
@@ -531,6 +525,12 @@
   </si>
   <si>
     <t>Apply for job</t>
+  </si>
+  <si>
+    <t>If blank / contsinas any special characters / any numeric values. Display an error message " Enter valid suburb"</t>
+  </si>
+  <si>
+    <t>After data stored in the database. An E-mail should be sent to Job seeker's E-mail ID. Job seeker should navigate to profile page</t>
   </si>
 </sst>
 </file>
@@ -620,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -671,11 +671,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -979,20 +982,20 @@
   <dimension ref="A1:I135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D62" sqref="D62"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="59.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="15" customWidth="1"/>
     <col min="7" max="7" width="7.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1001,7 +1004,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>12</v>
@@ -1027,9 +1030,11 @@
     </row>
     <row r="2" spans="1:9" s="10" customFormat="1">
       <c r="A2" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="11"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="14"/>
     </row>
@@ -1040,14 +1045,14 @@
       <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>21</v>
@@ -1063,24 +1068,26 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" ht="75">
-      <c r="A5" s="19" t="s">
-        <v>116</v>
+      <c r="A5" s="20" t="s">
+        <v>114</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F5" s="5">
         <v>30</v>
@@ -1096,18 +1103,18 @@
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" ht="75">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="2">
         <v>2</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F6" s="5">
         <v>30</v>
@@ -1123,18 +1130,18 @@
       </c>
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" ht="30">
-      <c r="A7" s="19"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="2">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F7" s="5">
         <v>30</v>
@@ -1150,18 +1157,18 @@
       </c>
     </row>
     <row r="8" spans="1:9" s="2" customFormat="1" ht="30">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="2">
         <v>4</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F8" s="5">
         <v>30</v>
@@ -1177,18 +1184,18 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="30">
-      <c r="A9" s="19"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="2">
         <v>5</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9" s="5">
         <v>30</v>
@@ -1204,18 +1211,18 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="60">
-      <c r="A10" s="19"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="18">
         <v>6</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F10" s="16">
         <v>30</v>
@@ -1231,18 +1238,18 @@
       </c>
     </row>
     <row r="11" spans="1:9" s="2" customFormat="1" ht="30">
-      <c r="A11" s="19"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="18">
         <v>7</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F11" s="16">
         <v>30</v>
@@ -1258,18 +1265,18 @@
       </c>
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" ht="45">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="2">
         <v>8</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F12" s="16">
         <v>10</v>
@@ -1285,18 +1292,18 @@
       </c>
     </row>
     <row r="13" spans="1:9" s="2" customFormat="1">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="18">
         <v>9</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F13" s="16">
         <v>30</v>
@@ -1311,19 +1318,19 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" ht="75">
-      <c r="A14" s="19"/>
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="30">
+      <c r="A14" s="20"/>
       <c r="B14" s="2">
         <v>10</v>
       </c>
-      <c r="C14" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>36</v>
+      <c r="C14" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="F14" s="5">
         <v>30</v>
@@ -1331,26 +1338,26 @@
       <c r="G14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>117</v>
+      <c r="H14" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="2" customFormat="1" ht="30">
-      <c r="A15" s="19"/>
+    <row r="15" spans="1:9" s="2" customFormat="1" ht="75">
+      <c r="A15" s="20"/>
       <c r="B15" s="2">
         <v>11</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F15" s="5">
         <v>30</v>
@@ -1358,26 +1365,26 @@
       <c r="G15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>21</v>
+      <c r="H15" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="2" customFormat="1" ht="30">
-      <c r="A16" s="19"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="2">
         <v>12</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F16" s="5">
         <v>4</v>
@@ -1393,24 +1400,24 @@
       </c>
     </row>
     <row r="17" spans="1:9" s="2" customFormat="1" ht="45">
-      <c r="A17" s="19"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="18">
         <v>13</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H17" s="18" t="s">
         <v>21</v>
@@ -1420,18 +1427,18 @@
       </c>
     </row>
     <row r="18" spans="1:9" s="2" customFormat="1" ht="45">
-      <c r="A18" s="19"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="18">
         <v>14</v>
       </c>
-      <c r="C18" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="D18" s="18" t="s">
+      <c r="C18" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F18" s="16">
         <v>50</v>
@@ -1447,18 +1454,18 @@
       </c>
     </row>
     <row r="19" spans="1:9" s="18" customFormat="1" ht="30">
-      <c r="A19" s="19"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="18">
         <v>15</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="F19" s="16" t="s">
         <v>21</v>
@@ -1474,18 +1481,18 @@
       </c>
     </row>
     <row r="20" spans="1:9" s="18" customFormat="1" ht="30">
-      <c r="A20" s="19"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="18">
         <v>16</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="18" t="s">
-        <v>99</v>
+      <c r="D20" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>21</v>
@@ -1501,18 +1508,18 @@
       </c>
     </row>
     <row r="21" spans="1:9" s="18" customFormat="1" ht="30">
-      <c r="A21" s="19"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="18">
         <v>17</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="3" t="s">
         <v>38</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F21" s="16">
         <v>1</v>
@@ -1528,18 +1535,18 @@
       </c>
     </row>
     <row r="22" spans="1:9" s="2" customFormat="1" ht="90">
-      <c r="A22" s="19"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="18">
         <v>18</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="20" t="s">
-        <v>106</v>
+      <c r="E22" s="19" t="s">
+        <v>104</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>21</v>
@@ -1556,6 +1563,8 @@
     </row>
     <row r="23" spans="1:9" s="2" customFormat="1">
       <c r="A23" s="4"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="5"/>
     </row>
@@ -1566,14 +1575,14 @@
       <c r="B24" s="2">
         <v>1</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>21</v>
@@ -1589,6 +1598,8 @@
       </c>
     </row>
     <row r="25" spans="1:9" s="2" customFormat="1">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="5"/>
     </row>
@@ -1599,14 +1610,14 @@
       <c r="B26" s="2">
         <v>1</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>21</v>
@@ -1622,6 +1633,8 @@
       </c>
     </row>
     <row r="27" spans="1:9" s="2" customFormat="1">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="5"/>
     </row>
@@ -1632,14 +1645,14 @@
       <c r="B28" s="2">
         <v>1</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>43</v>
+        <v>118</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>21</v>
@@ -1655,40 +1668,42 @@
       </c>
     </row>
     <row r="29" spans="1:9" s="2" customFormat="1">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:9" s="2" customFormat="1" ht="45">
-      <c r="A30" s="19" t="s">
-        <v>48</v>
+      <c r="A30" s="20" t="s">
+        <v>47</v>
       </c>
       <c r="B30" s="2">
         <v>1</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="C30" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:9" s="2" customFormat="1">
-      <c r="A31" s="19"/>
+      <c r="A31" s="20"/>
       <c r="B31" s="2">
         <v>1</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>21</v>
@@ -1704,38 +1719,40 @@
       </c>
     </row>
     <row r="32" spans="1:9" s="2" customFormat="1">
-      <c r="A32" s="19"/>
+      <c r="A32" s="20"/>
       <c r="B32" s="2">
         <v>2</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" s="2" customFormat="1" ht="30">
-      <c r="A33" s="19"/>
+      <c r="A33" s="20"/>
       <c r="B33" s="2">
         <v>3</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="2" t="s">
+      <c r="C33" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" s="2" customFormat="1">
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="5"/>
     </row>
@@ -1746,18 +1763,20 @@
       <c r="B35" s="2">
         <v>1</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>47</v>
+      <c r="C35" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" s="2" customFormat="1">
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="5"/>
     </row>
@@ -1768,18 +1787,20 @@
       <c r="B37" s="2">
         <v>1</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="C37" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" s="2" customFormat="1">
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="5"/>
     </row>
@@ -1790,18 +1811,20 @@
       <c r="B39" s="2">
         <v>1</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" s="2" customFormat="1">
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="5"/>
     </row>
@@ -1812,29 +1835,35 @@
       <c r="B41" s="2">
         <v>1</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:6" s="2" customFormat="1">
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:6" s="2" customFormat="1">
       <c r="A43" s="13" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="5"/>
     </row>
     <row r="44" spans="1:6" s="2" customFormat="1">
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="5"/>
     </row>
@@ -1845,18 +1874,20 @@
       <c r="B45" s="2">
         <v>1</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D45" s="2" t="s">
+      <c r="C45" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:6" s="2" customFormat="1">
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="5"/>
     </row>
@@ -1867,14 +1898,14 @@
       <c r="B47" s="2">
         <v>1</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="C47" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>24</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F47" s="5"/>
     </row>
@@ -1882,14 +1913,14 @@
       <c r="B48" s="2">
         <v>2</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D48" s="2" t="s">
+      <c r="C48" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F48" s="5"/>
     </row>
@@ -1897,14 +1928,14 @@
       <c r="B49" s="2">
         <v>3</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D49" s="2" t="s">
+      <c r="C49" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F49" s="5"/>
     </row>
@@ -1912,14 +1943,14 @@
       <c r="B50" s="2">
         <v>4</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D50" s="2" t="s">
+      <c r="C50" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F50" s="5"/>
     </row>
@@ -1927,14 +1958,14 @@
       <c r="B51" s="2">
         <v>5</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D51" s="2" t="s">
+      <c r="C51" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F51" s="5"/>
     </row>
@@ -1942,14 +1973,14 @@
       <c r="B52" s="2">
         <v>6</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D52" s="2" t="s">
+      <c r="C52" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F52" s="5"/>
     </row>
@@ -1957,14 +1988,14 @@
       <c r="B53" s="2">
         <v>7</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D53" s="2" t="s">
+      <c r="C53" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F53" s="5"/>
     </row>
@@ -1972,18 +2003,20 @@
       <c r="B54" s="2">
         <v>8</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D54" s="2" t="s">
+      <c r="C54" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F54" s="5"/>
     </row>
     <row r="55" spans="1:6" s="2" customFormat="1">
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
       <c r="E55" s="3"/>
       <c r="F55" s="5"/>
     </row>
@@ -1994,29 +2027,29 @@
       <c r="B56" s="2">
         <v>1</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>102</v>
+      <c r="C56" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F56" s="5"/>
     </row>
-    <row r="57" spans="1:6" s="2" customFormat="1">
+    <row r="57" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="B57" s="2">
         <v>2</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="F57" s="5"/>
     </row>
@@ -2024,29 +2057,35 @@
       <c r="B58" s="2">
         <v>3</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>102</v>
+      <c r="C58" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F58" s="5"/>
     </row>
     <row r="59" spans="1:6" s="2" customFormat="1">
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="5"/>
     </row>
     <row r="60" spans="1:6" s="2" customFormat="1">
       <c r="A60" s="13" t="s">
-        <v>103</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="5"/>
     </row>
     <row r="61" spans="1:6" s="2" customFormat="1">
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="5"/>
     </row>
@@ -2057,297 +2096,438 @@
       <c r="B62" s="2">
         <v>1</v>
       </c>
-      <c r="C62" s="18" t="s">
-        <v>118</v>
-      </c>
+      <c r="C62" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="5"/>
     </row>
     <row r="63" spans="1:6" s="2" customFormat="1">
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:6" s="2" customFormat="1">
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="5"/>
     </row>
-    <row r="65" spans="5:6" s="2" customFormat="1">
+    <row r="65" spans="3:6" s="2" customFormat="1">
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="5"/>
     </row>
-    <row r="66" spans="5:6" s="2" customFormat="1">
+    <row r="66" spans="3:6" s="2" customFormat="1">
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="5"/>
     </row>
-    <row r="67" spans="5:6" s="2" customFormat="1">
+    <row r="67" spans="3:6" s="2" customFormat="1">
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="5"/>
     </row>
-    <row r="68" spans="5:6" s="2" customFormat="1">
+    <row r="68" spans="3:6" s="2" customFormat="1">
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="5"/>
     </row>
-    <row r="69" spans="5:6" s="2" customFormat="1">
+    <row r="69" spans="3:6" s="2" customFormat="1">
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="5"/>
     </row>
-    <row r="70" spans="5:6" s="2" customFormat="1">
+    <row r="70" spans="3:6" s="2" customFormat="1">
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="5"/>
     </row>
-    <row r="71" spans="5:6" s="2" customFormat="1">
+    <row r="71" spans="3:6" s="2" customFormat="1">
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
       <c r="E71" s="3"/>
       <c r="F71" s="5"/>
     </row>
-    <row r="72" spans="5:6" s="2" customFormat="1">
+    <row r="72" spans="3:6" s="2" customFormat="1">
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="5"/>
     </row>
-    <row r="73" spans="5:6" s="2" customFormat="1">
+    <row r="73" spans="3:6" s="2" customFormat="1">
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="5"/>
     </row>
-    <row r="74" spans="5:6" s="2" customFormat="1">
+    <row r="74" spans="3:6" s="2" customFormat="1">
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="5"/>
     </row>
-    <row r="75" spans="5:6" s="2" customFormat="1">
+    <row r="75" spans="3:6" s="2" customFormat="1">
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
       <c r="E75" s="3"/>
       <c r="F75" s="5"/>
     </row>
-    <row r="76" spans="5:6" s="2" customFormat="1">
+    <row r="76" spans="3:6" s="2" customFormat="1">
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
       <c r="E76" s="3"/>
       <c r="F76" s="5"/>
     </row>
-    <row r="77" spans="5:6" s="2" customFormat="1">
+    <row r="77" spans="3:6" s="2" customFormat="1">
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
       <c r="E77" s="3"/>
       <c r="F77" s="5"/>
     </row>
-    <row r="78" spans="5:6" s="2" customFormat="1">
+    <row r="78" spans="3:6" s="2" customFormat="1">
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
       <c r="E78" s="3"/>
       <c r="F78" s="5"/>
     </row>
-    <row r="79" spans="5:6" s="2" customFormat="1">
+    <row r="79" spans="3:6" s="2" customFormat="1">
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
       <c r="E79" s="3"/>
       <c r="F79" s="5"/>
     </row>
-    <row r="80" spans="5:6" s="2" customFormat="1">
+    <row r="80" spans="3:6" s="2" customFormat="1">
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="5"/>
     </row>
-    <row r="81" spans="5:6" s="2" customFormat="1">
+    <row r="81" spans="3:6" s="2" customFormat="1">
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
       <c r="E81" s="3"/>
       <c r="F81" s="5"/>
     </row>
-    <row r="82" spans="5:6" s="2" customFormat="1">
+    <row r="82" spans="3:6" s="2" customFormat="1">
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
       <c r="E82" s="3"/>
       <c r="F82" s="5"/>
     </row>
-    <row r="83" spans="5:6" s="2" customFormat="1">
+    <row r="83" spans="3:6" s="2" customFormat="1">
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
       <c r="E83" s="3"/>
       <c r="F83" s="5"/>
     </row>
-    <row r="84" spans="5:6" s="2" customFormat="1">
+    <row r="84" spans="3:6" s="2" customFormat="1">
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
       <c r="E84" s="3"/>
       <c r="F84" s="5"/>
     </row>
-    <row r="85" spans="5:6" s="2" customFormat="1">
+    <row r="85" spans="3:6" s="2" customFormat="1">
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
       <c r="E85" s="3"/>
       <c r="F85" s="5"/>
     </row>
-    <row r="86" spans="5:6" s="2" customFormat="1">
+    <row r="86" spans="3:6" s="2" customFormat="1">
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="5"/>
     </row>
-    <row r="87" spans="5:6" s="2" customFormat="1">
+    <row r="87" spans="3:6" s="2" customFormat="1">
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
       <c r="E87" s="3"/>
       <c r="F87" s="5"/>
     </row>
-    <row r="88" spans="5:6" s="2" customFormat="1">
+    <row r="88" spans="3:6" s="2" customFormat="1">
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
       <c r="E88" s="3"/>
       <c r="F88" s="5"/>
     </row>
-    <row r="89" spans="5:6" s="2" customFormat="1">
+    <row r="89" spans="3:6" s="2" customFormat="1">
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="5"/>
     </row>
-    <row r="90" spans="5:6" s="2" customFormat="1">
+    <row r="90" spans="3:6" s="2" customFormat="1">
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="5"/>
     </row>
-    <row r="91" spans="5:6" s="2" customFormat="1">
+    <row r="91" spans="3:6" s="2" customFormat="1">
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="5"/>
     </row>
-    <row r="92" spans="5:6" s="2" customFormat="1">
+    <row r="92" spans="3:6" s="2" customFormat="1">
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
       <c r="E92" s="3"/>
       <c r="F92" s="5"/>
     </row>
-    <row r="93" spans="5:6" s="2" customFormat="1">
+    <row r="93" spans="3:6" s="2" customFormat="1">
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="5"/>
     </row>
-    <row r="94" spans="5:6" s="2" customFormat="1">
+    <row r="94" spans="3:6" s="2" customFormat="1">
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
       <c r="E94" s="3"/>
       <c r="F94" s="5"/>
     </row>
-    <row r="95" spans="5:6" s="2" customFormat="1">
+    <row r="95" spans="3:6" s="2" customFormat="1">
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
       <c r="E95" s="3"/>
       <c r="F95" s="5"/>
     </row>
-    <row r="96" spans="5:6" s="2" customFormat="1">
+    <row r="96" spans="3:6" s="2" customFormat="1">
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
       <c r="E96" s="3"/>
       <c r="F96" s="5"/>
     </row>
-    <row r="97" spans="5:6" s="2" customFormat="1">
+    <row r="97" spans="3:6" s="2" customFormat="1">
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
       <c r="E97" s="3"/>
       <c r="F97" s="5"/>
     </row>
-    <row r="98" spans="5:6" s="2" customFormat="1">
+    <row r="98" spans="3:6" s="2" customFormat="1">
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
       <c r="E98" s="3"/>
       <c r="F98" s="5"/>
     </row>
-    <row r="99" spans="5:6" s="2" customFormat="1">
+    <row r="99" spans="3:6" s="2" customFormat="1">
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
       <c r="E99" s="3"/>
       <c r="F99" s="5"/>
     </row>
-    <row r="100" spans="5:6" s="2" customFormat="1">
+    <row r="100" spans="3:6" s="2" customFormat="1">
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
       <c r="E100" s="3"/>
       <c r="F100" s="5"/>
     </row>
-    <row r="101" spans="5:6" s="2" customFormat="1">
+    <row r="101" spans="3:6" s="2" customFormat="1">
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
       <c r="E101" s="3"/>
       <c r="F101" s="5"/>
     </row>
-    <row r="102" spans="5:6" s="2" customFormat="1">
+    <row r="102" spans="3:6" s="2" customFormat="1">
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
       <c r="E102" s="3"/>
       <c r="F102" s="5"/>
     </row>
-    <row r="103" spans="5:6" s="2" customFormat="1">
+    <row r="103" spans="3:6" s="2" customFormat="1">
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
       <c r="E103" s="3"/>
       <c r="F103" s="5"/>
     </row>
-    <row r="104" spans="5:6" s="2" customFormat="1">
+    <row r="104" spans="3:6" s="2" customFormat="1">
+      <c r="C104" s="3"/>
+      <c r="D104" s="3"/>
       <c r="E104" s="3"/>
       <c r="F104" s="5"/>
     </row>
-    <row r="105" spans="5:6" s="2" customFormat="1">
+    <row r="105" spans="3:6" s="2" customFormat="1">
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
       <c r="E105" s="3"/>
       <c r="F105" s="5"/>
     </row>
-    <row r="106" spans="5:6" s="2" customFormat="1">
+    <row r="106" spans="3:6" s="2" customFormat="1">
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
       <c r="E106" s="3"/>
       <c r="F106" s="5"/>
     </row>
-    <row r="107" spans="5:6" s="2" customFormat="1">
+    <row r="107" spans="3:6" s="2" customFormat="1">
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
       <c r="E107" s="3"/>
       <c r="F107" s="5"/>
     </row>
-    <row r="108" spans="5:6" s="2" customFormat="1">
+    <row r="108" spans="3:6" s="2" customFormat="1">
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
       <c r="E108" s="3"/>
       <c r="F108" s="5"/>
     </row>
-    <row r="109" spans="5:6" s="2" customFormat="1">
+    <row r="109" spans="3:6" s="2" customFormat="1">
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
       <c r="E109" s="3"/>
       <c r="F109" s="5"/>
     </row>
-    <row r="110" spans="5:6" s="2" customFormat="1">
+    <row r="110" spans="3:6" s="2" customFormat="1">
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
       <c r="E110" s="3"/>
       <c r="F110" s="5"/>
     </row>
-    <row r="111" spans="5:6" s="2" customFormat="1">
+    <row r="111" spans="3:6" s="2" customFormat="1">
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
       <c r="E111" s="3"/>
       <c r="F111" s="5"/>
     </row>
-    <row r="112" spans="5:6" s="2" customFormat="1">
+    <row r="112" spans="3:6" s="2" customFormat="1">
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
       <c r="E112" s="3"/>
       <c r="F112" s="5"/>
     </row>
-    <row r="113" spans="5:6" s="2" customFormat="1">
+    <row r="113" spans="3:6" s="2" customFormat="1">
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
       <c r="E113" s="3"/>
       <c r="F113" s="5"/>
     </row>
-    <row r="114" spans="5:6" s="2" customFormat="1">
+    <row r="114" spans="3:6" s="2" customFormat="1">
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
       <c r="E114" s="3"/>
       <c r="F114" s="5"/>
     </row>
-    <row r="115" spans="5:6" s="2" customFormat="1">
+    <row r="115" spans="3:6" s="2" customFormat="1">
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
       <c r="E115" s="3"/>
       <c r="F115" s="5"/>
     </row>
-    <row r="116" spans="5:6" s="2" customFormat="1">
+    <row r="116" spans="3:6" s="2" customFormat="1">
+      <c r="C116" s="3"/>
+      <c r="D116" s="3"/>
       <c r="E116" s="3"/>
       <c r="F116" s="5"/>
     </row>
-    <row r="117" spans="5:6" s="2" customFormat="1">
+    <row r="117" spans="3:6" s="2" customFormat="1">
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
       <c r="E117" s="3"/>
       <c r="F117" s="5"/>
     </row>
-    <row r="118" spans="5:6" s="2" customFormat="1">
+    <row r="118" spans="3:6" s="2" customFormat="1">
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
       <c r="E118" s="3"/>
       <c r="F118" s="5"/>
     </row>
-    <row r="119" spans="5:6" s="2" customFormat="1">
+    <row r="119" spans="3:6" s="2" customFormat="1">
+      <c r="C119" s="3"/>
+      <c r="D119" s="3"/>
       <c r="E119" s="3"/>
       <c r="F119" s="5"/>
     </row>
-    <row r="120" spans="5:6" s="2" customFormat="1">
+    <row r="120" spans="3:6" s="2" customFormat="1">
+      <c r="C120" s="3"/>
+      <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="5"/>
     </row>
-    <row r="121" spans="5:6" s="2" customFormat="1">
+    <row r="121" spans="3:6" s="2" customFormat="1">
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
       <c r="E121" s="3"/>
       <c r="F121" s="5"/>
     </row>
-    <row r="122" spans="5:6" s="2" customFormat="1">
+    <row r="122" spans="3:6" s="2" customFormat="1">
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
       <c r="E122" s="3"/>
       <c r="F122" s="5"/>
     </row>
-    <row r="123" spans="5:6" s="2" customFormat="1">
+    <row r="123" spans="3:6" s="2" customFormat="1">
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
       <c r="E123" s="3"/>
       <c r="F123" s="5"/>
     </row>
-    <row r="124" spans="5:6" s="2" customFormat="1">
+    <row r="124" spans="3:6" s="2" customFormat="1">
+      <c r="C124" s="3"/>
+      <c r="D124" s="3"/>
       <c r="E124" s="3"/>
       <c r="F124" s="5"/>
     </row>
-    <row r="125" spans="5:6" s="2" customFormat="1">
+    <row r="125" spans="3:6" s="2" customFormat="1">
+      <c r="C125" s="3"/>
+      <c r="D125" s="3"/>
       <c r="E125" s="3"/>
       <c r="F125" s="5"/>
     </row>
-    <row r="126" spans="5:6" s="2" customFormat="1">
+    <row r="126" spans="3:6" s="2" customFormat="1">
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
       <c r="E126" s="3"/>
       <c r="F126" s="5"/>
     </row>
-    <row r="127" spans="5:6" s="2" customFormat="1">
+    <row r="127" spans="3:6" s="2" customFormat="1">
+      <c r="C127" s="3"/>
+      <c r="D127" s="3"/>
       <c r="E127" s="3"/>
       <c r="F127" s="5"/>
     </row>
-    <row r="128" spans="5:6" s="2" customFormat="1">
+    <row r="128" spans="3:6" s="2" customFormat="1">
+      <c r="C128" s="3"/>
+      <c r="D128" s="3"/>
       <c r="E128" s="3"/>
       <c r="F128" s="5"/>
     </row>
     <row r="129" spans="1:9" s="2" customFormat="1">
+      <c r="C129" s="3"/>
+      <c r="D129" s="3"/>
       <c r="E129" s="3"/>
       <c r="F129" s="5"/>
     </row>
     <row r="130" spans="1:9" s="2" customFormat="1">
+      <c r="C130" s="3"/>
+      <c r="D130" s="3"/>
       <c r="E130" s="3"/>
       <c r="F130" s="5"/>
     </row>
     <row r="131" spans="1:9" s="2" customFormat="1">
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
       <c r="E131" s="3"/>
       <c r="F131" s="5"/>
     </row>
     <row r="132" spans="1:9" s="2" customFormat="1">
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
       <c r="E132" s="3"/>
       <c r="F132" s="5"/>
     </row>
     <row r="133" spans="1:9">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
-      <c r="C133" s="2"/>
-      <c r="D133" s="2"/>
+      <c r="C133" s="3"/>
+      <c r="D133" s="3"/>
       <c r="E133" s="3"/>
       <c r="F133" s="5"/>
       <c r="G133" s="2"/>
@@ -2357,8 +2537,8 @@
     <row r="134" spans="1:9">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
-      <c r="C134" s="2"/>
-      <c r="D134" s="2"/>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
       <c r="E134" s="3"/>
       <c r="F134" s="5"/>
       <c r="G134" s="2"/>
@@ -2368,8 +2548,8 @@
     <row r="135" spans="1:9">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
-      <c r="C135" s="2"/>
-      <c r="D135" s="2"/>
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
       <c r="E135" s="3"/>
       <c r="F135" s="5"/>
       <c r="G135" s="2"/>

</xml_diff>